<commit_message>
Latest version of bcl2fastq
</commit_message>
<xml_diff>
--- a/summaries/longContigSampleSummary_gte90percentRef.xlsx
+++ b/summaries/longContigSampleSummary_gte90percentRef.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -56,7 +56,7 @@
     <t xml:space="preserve">ETA</t>
   </si>
   <si>
-    <t xml:space="preserve">3/30/2020</t>
+    <t xml:space="preserve">03/30/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200330</t>
@@ -68,7 +68,7 @@
     <t xml:space="preserve">VSP0010</t>
   </si>
   <si>
-    <t xml:space="preserve">4/8/2020</t>
+    <t xml:space="preserve">04/08/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200408</t>
@@ -104,18 +104,12 @@
     <t xml:space="preserve">VSP0013</t>
   </si>
   <si>
-    <t xml:space="preserve">4/13/2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">VSP0184</t>
   </si>
   <si>
     <t xml:space="preserve">NP</t>
   </si>
   <si>
-    <t xml:space="preserve">04/08/2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">VSP0185</t>
   </si>
   <si>
@@ -128,7 +122,7 @@
     <t xml:space="preserve">VSP0014</t>
   </si>
   <si>
-    <t xml:space="preserve">4/15/2020</t>
+    <t xml:space="preserve">04/15/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200415</t>
@@ -170,7 +164,7 @@
     <t xml:space="preserve">VSP0020</t>
   </si>
   <si>
-    <t xml:space="preserve">4/22/2020</t>
+    <t xml:space="preserve">04/22/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200422</t>
@@ -224,7 +218,7 @@
     <t xml:space="preserve">VSP0033</t>
   </si>
   <si>
-    <t xml:space="preserve">4/27/2020</t>
+    <t xml:space="preserve">04/27/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200427</t>
@@ -233,7 +227,7 @@
     <t xml:space="preserve">VSP0038</t>
   </si>
   <si>
-    <t xml:space="preserve">4/29/2020</t>
+    <t xml:space="preserve">04/29/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200429</t>
@@ -248,7 +242,7 @@
     <t xml:space="preserve">239</t>
   </si>
   <si>
-    <t xml:space="preserve">VSP0041-2</t>
+    <t xml:space="preserve">VSP0041</t>
   </si>
   <si>
     <t xml:space="preserve">VSP0042</t>
@@ -359,27 +353,27 @@
     <t xml:space="preserve">266</t>
   </si>
   <si>
+    <t xml:space="preserve">VSP0320-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/22/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200522</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0262-1</t>
   </si>
   <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">5/20/20</t>
+    <t xml:space="preserve">Unk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/20/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200520</t>
   </si>
   <si>
-    <t xml:space="preserve">VSP0320-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5/22/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200522</t>
-  </si>
-  <si>
     <t xml:space="preserve">269</t>
   </si>
   <si>
@@ -404,9 +398,6 @@
     <t xml:space="preserve">VSP0166-1</t>
   </si>
   <si>
-    <t xml:space="preserve">05/22/2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">272</t>
   </si>
   <si>
@@ -443,7 +434,7 @@
     <t xml:space="preserve">Vero cells</t>
   </si>
   <si>
-    <t xml:space="preserve">3/28/2020</t>
+    <t xml:space="preserve">03/28/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200328</t>
@@ -981,7 +972,7 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G7" t="n">
         <v>29.9</v>
@@ -1001,17 +992,17 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="G8" t="n">
         <v>29.86</v>
@@ -1031,14 +1022,14 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
         <v>27</v>
@@ -1058,10 +1049,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -1071,7 +1062,7 @@
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G10" t="n">
         <v>29.86</v>
@@ -1083,25 +1074,25 @@
         <v>99.7</v>
       </c>
       <c r="J10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G11" t="n">
         <v>29.87</v>
@@ -1113,25 +1104,25 @@
         <v>99.7</v>
       </c>
       <c r="J11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G12" t="n">
         <v>29.34</v>
@@ -1143,25 +1134,25 @@
         <v>99.9</v>
       </c>
       <c r="J12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G13" t="n">
         <v>29.88</v>
@@ -1173,25 +1164,25 @@
         <v>99.9</v>
       </c>
       <c r="J13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G14" t="n">
         <v>29.96</v>
@@ -1203,28 +1194,28 @@
         <v>99.9</v>
       </c>
       <c r="J14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G15" t="n">
-        <v>29.98</v>
+        <v>29.91</v>
       </c>
       <c r="H15" t="n">
         <v>99.8</v>
@@ -1233,25 +1224,25 @@
         <v>99.8</v>
       </c>
       <c r="J15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G16" t="n">
         <v>29.82</v>
@@ -1263,25 +1254,25 @@
         <v>99.8</v>
       </c>
       <c r="J16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
         <v>54</v>
-      </c>
-      <c r="B17" t="s">
-        <v>56</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G17" t="n">
         <v>29.9</v>
@@ -1293,25 +1284,25 @@
         <v>99.8</v>
       </c>
       <c r="J17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G18" t="n">
         <v>29.68</v>
@@ -1323,27 +1314,27 @@
         <v>98.8</v>
       </c>
       <c r="J18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" t="n">
         <v>85100</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G19" t="n">
         <v>29.82</v>
@@ -1355,27 +1346,27 @@
         <v>99.8</v>
       </c>
       <c r="J19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D20" t="n">
         <v>176000</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G20" t="n">
         <v>29.87</v>
@@ -1387,25 +1378,25 @@
         <v>99.8</v>
       </c>
       <c r="J20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G21" t="n">
         <v>29.97</v>
@@ -1417,25 +1408,25 @@
         <v>99.8</v>
       </c>
       <c r="J21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G22" t="n">
         <v>29.92</v>
@@ -1447,25 +1438,25 @@
         <v>99.5</v>
       </c>
       <c r="J22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G23" t="n">
         <v>29.89</v>
@@ -1477,55 +1468,55 @@
         <v>99.8</v>
       </c>
       <c r="J23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G24" t="n">
-        <v>30.13</v>
+        <v>30.06</v>
       </c>
       <c r="H24" t="n">
-        <v>99.8</v>
+        <v>99.9</v>
       </c>
       <c r="I24" t="n">
-        <v>99.5</v>
+        <v>99.8</v>
       </c>
       <c r="J24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s">
         <v>77</v>
-      </c>
-      <c r="B25" t="s">
-        <v>79</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G25" t="n">
         <v>27.48</v>
@@ -1537,27 +1528,27 @@
         <v>99.8</v>
       </c>
       <c r="J25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D26" t="n">
         <v>364000</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G26" t="n">
         <v>29.45</v>
@@ -1569,18 +1560,18 @@
         <v>99.8</v>
       </c>
       <c r="J26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D27" t="n">
         <v>1420000</v>
@@ -1589,7 +1580,7 @@
         <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G27" t="n">
         <v>29.31</v>
@@ -1601,25 +1592,25 @@
         <v>99.7</v>
       </c>
       <c r="J27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G28" t="n">
         <v>29.88</v>
@@ -1631,27 +1622,27 @@
         <v>99.8</v>
       </c>
       <c r="J28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D29" t="n">
         <v>222000</v>
       </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G29" t="n">
         <v>29.89</v>
@@ -1663,27 +1654,27 @@
         <v>99.8</v>
       </c>
       <c r="J29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D30" t="n">
         <v>667</v>
       </c>
       <c r="E30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G30" t="n">
         <v>29.72</v>
@@ -1695,18 +1686,18 @@
         <v>99.2</v>
       </c>
       <c r="J30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D31" t="n">
         <v>255500</v>
@@ -1715,10 +1706,10 @@
         <v>13</v>
       </c>
       <c r="F31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G31" t="n">
-        <v>29.87</v>
+        <v>29.82</v>
       </c>
       <c r="H31" t="n">
         <v>99.8</v>
@@ -1727,25 +1718,25 @@
         <v>99.8</v>
       </c>
       <c r="J31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
       </c>
       <c r="D32"/>
       <c r="E32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G32" t="n">
         <v>29.94</v>
@@ -1757,25 +1748,25 @@
         <v>99.8</v>
       </c>
       <c r="J32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
       </c>
       <c r="D33"/>
       <c r="E33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G33" t="n">
         <v>30</v>
@@ -1787,18 +1778,18 @@
         <v>99.7</v>
       </c>
       <c r="J33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B34" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D34" t="n">
         <v>2760000</v>
@@ -1807,7 +1798,7 @@
         <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G34" t="n">
         <v>29.82</v>
@@ -1819,18 +1810,18 @@
         <v>99.7</v>
       </c>
       <c r="J34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D35" t="n">
         <v>123000</v>
@@ -1839,7 +1830,7 @@
         <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G35" t="n">
         <v>29.89</v>
@@ -1851,28 +1842,28 @@
         <v>99.8</v>
       </c>
       <c r="J35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
       </c>
       <c r="D36"/>
       <c r="E36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F36" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G36" t="n">
-        <v>30.07</v>
+        <v>29.99</v>
       </c>
       <c r="H36" t="n">
         <v>99.9</v>
@@ -1881,27 +1872,27 @@
         <v>99.9</v>
       </c>
       <c r="J36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D37" t="n">
         <v>51800</v>
       </c>
       <c r="E37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G37" t="n">
         <v>29.93</v>
@@ -1913,25 +1904,25 @@
         <v>99.8</v>
       </c>
       <c r="J37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D38"/>
       <c r="E38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G38" t="n">
         <v>29.82</v>
@@ -1943,28 +1934,28 @@
         <v>99.7</v>
       </c>
       <c r="J38" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D39"/>
       <c r="E39" t="s">
         <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G39" t="n">
-        <v>29.86</v>
+        <v>29.81</v>
       </c>
       <c r="H39" t="n">
         <v>99.7</v>
@@ -1973,27 +1964,27 @@
         <v>99.6</v>
       </c>
       <c r="J39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" t="s">
         <v>111</v>
       </c>
-      <c r="B40" t="s">
-        <v>113</v>
-      </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D40" t="n">
         <v>172000</v>
       </c>
       <c r="E40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G40" t="n">
         <v>29.85</v>
@@ -2005,78 +1996,78 @@
         <v>99.8</v>
       </c>
       <c r="J40" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D41"/>
       <c r="E41" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="F41" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G41" t="n">
-        <v>29.98</v>
+        <v>29.86</v>
       </c>
       <c r="H41" t="n">
-        <v>99.9</v>
+        <v>99.8</v>
       </c>
       <c r="I41" t="n">
         <v>99.8</v>
       </c>
       <c r="J41" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D42"/>
       <c r="E42" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="F42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G42" t="n">
-        <v>29.86</v>
+        <v>29.98</v>
       </c>
       <c r="H42" t="n">
-        <v>99.8</v>
+        <v>99.9</v>
       </c>
       <c r="I42" t="n">
         <v>99.8</v>
       </c>
       <c r="J42" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D43" t="n">
         <v>166000</v>
@@ -2085,7 +2076,7 @@
         <v>13</v>
       </c>
       <c r="F43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G43" t="n">
         <v>29.82</v>
@@ -2097,18 +2088,18 @@
         <v>99.8</v>
       </c>
       <c r="J43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B44" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D44" t="n">
         <v>16300</v>
@@ -2117,7 +2108,7 @@
         <v>13</v>
       </c>
       <c r="F44" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G44" t="n">
         <v>29.83</v>
@@ -2129,25 +2120,25 @@
         <v>99.8</v>
       </c>
       <c r="J44" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C45" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D45"/>
       <c r="E45" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F45" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="G45" t="n">
         <v>29.84</v>
@@ -2159,27 +2150,27 @@
         <v>99.5</v>
       </c>
       <c r="J45" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D46" t="n">
         <v>14500</v>
       </c>
       <c r="E46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F46" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G46" t="n">
         <v>29.41</v>
@@ -2191,25 +2182,25 @@
         <v>99.8</v>
       </c>
       <c r="J46" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C47" t="s">
         <v>12</v>
       </c>
       <c r="D47"/>
       <c r="E47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F47" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G47" t="n">
         <v>29.8</v>
@@ -2221,27 +2212,27 @@
         <v>99.8</v>
       </c>
       <c r="J47" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B48" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C48" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D48" t="n">
         <v>27900</v>
       </c>
       <c r="E48" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F48" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G48" t="n">
         <v>29.91</v>
@@ -2253,25 +2244,25 @@
         <v>99.8</v>
       </c>
       <c r="J48" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B49" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C49" t="s">
         <v>12</v>
       </c>
       <c r="D49"/>
       <c r="E49" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F49" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G49" t="n">
         <v>27.21</v>
@@ -2283,25 +2274,25 @@
         <v>99.8</v>
       </c>
       <c r="J49" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
         <v>12</v>
       </c>
       <c r="D50"/>
       <c r="E50" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F50" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G50" t="n">
         <v>30.02</v>
@@ -2313,7 +2304,7 @@
         <v>99.8</v>
       </c>
       <c r="J50" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new high qual genome cutoff
</commit_message>
<xml_diff>
--- a/summaries/longContigSampleSummary_gte90percentRef.xlsx
+++ b/summaries/longContigSampleSummary_gte90percentRef.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -44,6 +44,9 @@
     <t xml:space="preserve">sampleDate2</t>
   </si>
   <si>
+    <t xml:space="preserve">sampleName</t>
+  </si>
+  <si>
     <t xml:space="preserve">197</t>
   </si>
   <si>
@@ -62,6 +65,9 @@
     <t xml:space="preserve">20200330</t>
   </si>
   <si>
+    <t xml:space="preserve">197 ETA 20200330</t>
+  </si>
+  <si>
     <t xml:space="preserve">203</t>
   </si>
   <si>
@@ -74,18 +80,27 @@
     <t xml:space="preserve">20200408</t>
   </si>
   <si>
+    <t xml:space="preserve">203 ETA 20200408</t>
+  </si>
+  <si>
     <t xml:space="preserve">209</t>
   </si>
   <si>
     <t xml:space="preserve">VSP0011</t>
   </si>
   <si>
+    <t xml:space="preserve">209 ETA 20200408</t>
+  </si>
+  <si>
     <t xml:space="preserve">210</t>
   </si>
   <si>
     <t xml:space="preserve">VSP0012</t>
   </si>
   <si>
+    <t xml:space="preserve">210 ETA 20200408</t>
+  </si>
+  <si>
     <t xml:space="preserve">211</t>
   </si>
   <si>
@@ -101,21 +116,33 @@
     <t xml:space="preserve">20200413</t>
   </si>
   <si>
+    <t xml:space="preserve">211 ET 20200413</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0013</t>
   </si>
   <si>
+    <t xml:space="preserve">211 ETA 20200413</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0184</t>
   </si>
   <si>
     <t xml:space="preserve">NP</t>
   </si>
   <si>
+    <t xml:space="preserve">211 NP 20200408</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0185</t>
   </si>
   <si>
     <t xml:space="preserve">OP</t>
   </si>
   <si>
+    <t xml:space="preserve">211 OP 20200413</t>
+  </si>
+  <si>
     <t xml:space="preserve">213</t>
   </si>
   <si>
@@ -128,6 +155,9 @@
     <t xml:space="preserve">20200415</t>
   </si>
   <si>
+    <t xml:space="preserve">213 ETA 20200415</t>
+  </si>
+  <si>
     <t xml:space="preserve">222</t>
   </si>
   <si>
@@ -140,9 +170,15 @@
     <t xml:space="preserve">20200417</t>
   </si>
   <si>
+    <t xml:space="preserve">222 NP 20200417</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0181</t>
   </si>
   <si>
+    <t xml:space="preserve">222 OP 20200417</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0182</t>
   </si>
   <si>
@@ -152,12 +188,18 @@
     <t xml:space="preserve">20200420</t>
   </si>
   <si>
+    <t xml:space="preserve">222 OP 20200420</t>
+  </si>
+  <si>
     <t xml:space="preserve">223</t>
   </si>
   <si>
     <t xml:space="preserve">VSP0183</t>
   </si>
   <si>
+    <t xml:space="preserve">223 OP 20200417</t>
+  </si>
+  <si>
     <t xml:space="preserve">227</t>
   </si>
   <si>
@@ -170,12 +212,18 @@
     <t xml:space="preserve">20200422</t>
   </si>
   <si>
+    <t xml:space="preserve">227 OP 20200422</t>
+  </si>
+  <si>
     <t xml:space="preserve">228</t>
   </si>
   <si>
     <t xml:space="preserve">VSP0021</t>
   </si>
   <si>
+    <t xml:space="preserve">228 NP 20200422</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0188</t>
   </si>
   <si>
@@ -188,9 +236,15 @@
     <t xml:space="preserve">20200529</t>
   </si>
   <si>
+    <t xml:space="preserve">228 NP-OP 20200529</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0022</t>
   </si>
   <si>
+    <t xml:space="preserve">228 OP 20200422</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0189-1</t>
   </si>
   <si>
@@ -200,6 +254,9 @@
     <t xml:space="preserve">Saliva</t>
   </si>
   <si>
+    <t xml:space="preserve">228 Saliva 20200529</t>
+  </si>
+  <si>
     <t xml:space="preserve">235</t>
   </si>
   <si>
@@ -212,6 +269,9 @@
     <t xml:space="preserve">20200424</t>
   </si>
   <si>
+    <t xml:space="preserve">235 NP-OP 20200424</t>
+  </si>
+  <si>
     <t xml:space="preserve">237</t>
   </si>
   <si>
@@ -224,6 +284,9 @@
     <t xml:space="preserve">20200427</t>
   </si>
   <si>
+    <t xml:space="preserve">237 NP-OP 20200427</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0038</t>
   </si>
   <si>
@@ -233,21 +296,33 @@
     <t xml:space="preserve">20200429</t>
   </si>
   <si>
+    <t xml:space="preserve">237 OP 20200429</t>
+  </si>
+  <si>
     <t xml:space="preserve">238</t>
   </si>
   <si>
     <t xml:space="preserve">VSP0039</t>
   </si>
   <si>
+    <t xml:space="preserve">238 NP 20200429</t>
+  </si>
+  <si>
     <t xml:space="preserve">239</t>
   </si>
   <si>
     <t xml:space="preserve">VSP0041</t>
   </si>
   <si>
+    <t xml:space="preserve">239 NP 20200429</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0042</t>
   </si>
   <si>
+    <t xml:space="preserve">239 OP 20200429</t>
+  </si>
+  <si>
     <t xml:space="preserve">240</t>
   </si>
   <si>
@@ -260,6 +335,9 @@
     <t xml:space="preserve">20200501</t>
   </si>
   <si>
+    <t xml:space="preserve">240 NP-OP 20200501</t>
+  </si>
+  <si>
     <t xml:space="preserve">242</t>
   </si>
   <si>
@@ -272,15 +350,27 @@
     <t xml:space="preserve">20200504</t>
   </si>
   <si>
+    <t xml:space="preserve">242 ETA 20200504</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0044</t>
   </si>
   <si>
+    <t xml:space="preserve">242 NP 20200429</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0047-1</t>
   </si>
   <si>
+    <t xml:space="preserve">242 NP-OP 20200501</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0045-1</t>
   </si>
   <si>
+    <t xml:space="preserve">242 OP 20200429</t>
+  </si>
+  <si>
     <t xml:space="preserve">251</t>
   </si>
   <si>
@@ -293,12 +383,21 @@
     <t xml:space="preserve">20200506</t>
   </si>
   <si>
+    <t xml:space="preserve">251 ETA 20200506</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0065</t>
   </si>
   <si>
+    <t xml:space="preserve">251 NP-OP 20200504</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0089</t>
   </si>
   <si>
+    <t xml:space="preserve">251 NP-OP 20200506</t>
+  </si>
+  <si>
     <t xml:space="preserve">256</t>
   </si>
   <si>
@@ -311,6 +410,9 @@
     <t xml:space="preserve">20200508</t>
   </si>
   <si>
+    <t xml:space="preserve">256 ETA 20200508</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0123-1</t>
   </si>
   <si>
@@ -320,15 +422,24 @@
     <t xml:space="preserve">20200511</t>
   </si>
   <si>
+    <t xml:space="preserve">256 ETA 20200511</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0107</t>
   </si>
   <si>
+    <t xml:space="preserve">256 NP-OP 20200508</t>
+  </si>
+  <si>
     <t xml:space="preserve">257</t>
   </si>
   <si>
     <t xml:space="preserve">VSP0102-1</t>
   </si>
   <si>
+    <t xml:space="preserve">257 NP-OP 20200508</t>
+  </si>
+  <si>
     <t xml:space="preserve">262</t>
   </si>
   <si>
@@ -341,15 +452,24 @@
     <t xml:space="preserve">20200515</t>
   </si>
   <si>
+    <t xml:space="preserve">262 NP-OP 20200515</t>
+  </si>
+  <si>
     <t xml:space="preserve">263</t>
   </si>
   <si>
     <t xml:space="preserve">VSP0142-1</t>
   </si>
   <si>
+    <t xml:space="preserve">263 ETA 20200515</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0143-1</t>
   </si>
   <si>
+    <t xml:space="preserve">263 NP-OP 20200515</t>
+  </si>
+  <si>
     <t xml:space="preserve">266</t>
   </si>
   <si>
@@ -362,6 +482,9 @@
     <t xml:space="preserve">20200522</t>
   </si>
   <si>
+    <t xml:space="preserve">266 NP-OP 20200522</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0262-1</t>
   </si>
   <si>
@@ -374,6 +497,9 @@
     <t xml:space="preserve">20200520</t>
   </si>
   <si>
+    <t xml:space="preserve">266 Unk 20200520</t>
+  </si>
+  <si>
     <t xml:space="preserve">269</t>
   </si>
   <si>
@@ -386,6 +512,9 @@
     <t xml:space="preserve">20200527</t>
   </si>
   <si>
+    <t xml:space="preserve">269 ETA 20200527</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0202-1</t>
   </si>
   <si>
@@ -395,15 +524,24 @@
     <t xml:space="preserve">20200612</t>
   </si>
   <si>
+    <t xml:space="preserve">269 ETA 20200612</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0166-1</t>
   </si>
   <si>
+    <t xml:space="preserve">269 NP-OP 20200522</t>
+  </si>
+  <si>
     <t xml:space="preserve">272</t>
   </si>
   <si>
     <t xml:space="preserve">VSP0179-1</t>
   </si>
   <si>
+    <t xml:space="preserve">272 NP-OP 20200527</t>
+  </si>
+  <si>
     <t xml:space="preserve">290</t>
   </si>
   <si>
@@ -416,6 +554,9 @@
     <t xml:space="preserve">20200629</t>
   </si>
   <si>
+    <t xml:space="preserve">290 NP-OP 20200629</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSP0233-2</t>
   </si>
   <si>
@@ -425,6 +566,9 @@
     <t xml:space="preserve">20200701</t>
   </si>
   <si>
+    <t xml:space="preserve">290 NP-OP 20200701</t>
+  </si>
+  <si>
     <t xml:space="preserve">CCLB</t>
   </si>
   <si>
@@ -440,10 +584,16 @@
     <t xml:space="preserve">20200328</t>
   </si>
   <si>
+    <t xml:space="preserve">CCLB Vero cells 20200328</t>
+  </si>
+  <si>
     <t xml:space="preserve">E6</t>
   </si>
   <si>
     <t xml:space="preserve">VSP0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E6 Vero cells 20200328</t>
   </si>
 </sst>
 </file>
@@ -806,23 +956,26 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="n">
         <v>29.82</v>
@@ -834,25 +987,28 @@
         <v>99.8</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G3" t="n">
         <v>29.84</v>
@@ -864,25 +1020,28 @@
         <v>99.4</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G4" t="n">
         <v>29.85</v>
@@ -894,25 +1053,28 @@
         <v>99.4</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G5" t="n">
         <v>29.86</v>
@@ -924,25 +1086,28 @@
         <v>99.7</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G6" t="n">
         <v>29.8</v>
@@ -954,25 +1119,28 @@
         <v>99.8</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G7" t="n">
         <v>29.9</v>
@@ -984,25 +1152,28 @@
         <v>99.8</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G8" t="n">
         <v>29.86</v>
@@ -1014,25 +1185,28 @@
         <v>99.8</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="K8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G9" t="n">
         <v>29.88</v>
@@ -1044,25 +1218,28 @@
         <v>99.8</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="K9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G10" t="n">
         <v>29.86</v>
@@ -1074,25 +1251,28 @@
         <v>99.7</v>
       </c>
       <c r="J10" t="s">
-        <v>37</v>
+        <v>46</v>
+      </c>
+      <c r="K10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G11" t="n">
         <v>29.87</v>
@@ -1104,25 +1284,28 @@
         <v>99.7</v>
       </c>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>51</v>
+      </c>
+      <c r="K11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G12" t="n">
         <v>29.34</v>
@@ -1134,25 +1317,28 @@
         <v>99.9</v>
       </c>
       <c r="J12" t="s">
-        <v>41</v>
+        <v>51</v>
+      </c>
+      <c r="K12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G13" t="n">
         <v>29.88</v>
@@ -1164,25 +1350,28 @@
         <v>99.9</v>
       </c>
       <c r="J13" t="s">
-        <v>45</v>
+        <v>57</v>
+      </c>
+      <c r="K13" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G14" t="n">
         <v>29.96</v>
@@ -1194,25 +1383,28 @@
         <v>99.9</v>
       </c>
       <c r="J14" t="s">
-        <v>41</v>
+        <v>51</v>
+      </c>
+      <c r="K14" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="G15" t="n">
         <v>29.91</v>
@@ -1224,25 +1416,28 @@
         <v>99.8</v>
       </c>
       <c r="J15" t="s">
-        <v>51</v>
+        <v>65</v>
+      </c>
+      <c r="K15" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="G16" t="n">
         <v>29.82</v>
@@ -1254,25 +1449,28 @@
         <v>99.8</v>
       </c>
       <c r="J16" t="s">
-        <v>51</v>
+        <v>65</v>
+      </c>
+      <c r="K16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="G17" t="n">
         <v>29.9</v>
@@ -1284,25 +1482,28 @@
         <v>99.8</v>
       </c>
       <c r="J17" t="s">
-        <v>57</v>
+        <v>73</v>
+      </c>
+      <c r="K17" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="G18" t="n">
         <v>29.68</v>
@@ -1314,27 +1515,30 @@
         <v>98.8</v>
       </c>
       <c r="J18" t="s">
-        <v>51</v>
+        <v>65</v>
+      </c>
+      <c r="K18" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D19" t="n">
         <v>85100</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="G19" t="n">
         <v>29.82</v>
@@ -1346,27 +1550,30 @@
         <v>99.8</v>
       </c>
       <c r="J19" t="s">
-        <v>57</v>
+        <v>73</v>
+      </c>
+      <c r="K19" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D20" t="n">
         <v>176000</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="G20" t="n">
         <v>29.87</v>
@@ -1378,25 +1585,28 @@
         <v>99.8</v>
       </c>
       <c r="J20" t="s">
-        <v>65</v>
+        <v>84</v>
+      </c>
+      <c r="K20" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="G21" t="n">
         <v>29.97</v>
@@ -1408,25 +1618,28 @@
         <v>99.8</v>
       </c>
       <c r="J21" t="s">
-        <v>69</v>
+        <v>89</v>
+      </c>
+      <c r="K21" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F22" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="G22" t="n">
         <v>29.92</v>
@@ -1438,25 +1651,28 @@
         <v>99.5</v>
       </c>
       <c r="J22" t="s">
-        <v>72</v>
+        <v>93</v>
+      </c>
+      <c r="K22" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="G23" t="n">
         <v>29.89</v>
@@ -1468,25 +1684,28 @@
         <v>99.8</v>
       </c>
       <c r="J23" t="s">
-        <v>72</v>
+        <v>93</v>
+      </c>
+      <c r="K23" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F24" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="G24" t="n">
         <v>30.06</v>
@@ -1498,25 +1717,28 @@
         <v>99.8</v>
       </c>
       <c r="J24" t="s">
-        <v>72</v>
+        <v>93</v>
+      </c>
+      <c r="K24" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F25" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="G25" t="n">
         <v>27.48</v>
@@ -1528,27 +1750,30 @@
         <v>99.8</v>
       </c>
       <c r="J25" t="s">
-        <v>72</v>
+        <v>93</v>
+      </c>
+      <c r="K25" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" t="s">
         <v>78</v>
-      </c>
-      <c r="B26" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" t="s">
-        <v>60</v>
       </c>
       <c r="D26" t="n">
         <v>364000</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F26" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="G26" t="n">
         <v>29.45</v>
@@ -1560,27 +1785,30 @@
         <v>99.8</v>
       </c>
       <c r="J26" t="s">
-        <v>81</v>
+        <v>106</v>
+      </c>
+      <c r="K26" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D27" t="n">
         <v>1420000</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G27" t="n">
         <v>29.31</v>
@@ -1592,25 +1820,28 @@
         <v>99.7</v>
       </c>
       <c r="J27" t="s">
-        <v>85</v>
+        <v>111</v>
+      </c>
+      <c r="K27" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F28" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="G28" t="n">
         <v>29.88</v>
@@ -1622,27 +1853,30 @@
         <v>99.8</v>
       </c>
       <c r="J28" t="s">
-        <v>72</v>
+        <v>93</v>
+      </c>
+      <c r="K28" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D29" t="n">
         <v>222000</v>
       </c>
       <c r="E29" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F29" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="G29" t="n">
         <v>29.89</v>
@@ -1654,27 +1888,30 @@
         <v>99.8</v>
       </c>
       <c r="J29" t="s">
-        <v>81</v>
+        <v>106</v>
+      </c>
+      <c r="K29" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D30" t="n">
         <v>667</v>
       </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F30" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="G30" t="n">
         <v>29.72</v>
@@ -1686,27 +1923,30 @@
         <v>99.2</v>
       </c>
       <c r="J30" t="s">
-        <v>72</v>
+        <v>93</v>
+      </c>
+      <c r="K30" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D31" t="n">
         <v>255500</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="G31" t="n">
         <v>29.82</v>
@@ -1718,25 +1958,28 @@
         <v>99.8</v>
       </c>
       <c r="J31" t="s">
-        <v>92</v>
+        <v>122</v>
+      </c>
+      <c r="K31" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="B32" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D32"/>
       <c r="E32" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F32" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="G32" t="n">
         <v>29.94</v>
@@ -1748,25 +1991,28 @@
         <v>99.8</v>
       </c>
       <c r="J32" t="s">
-        <v>85</v>
+        <v>111</v>
+      </c>
+      <c r="K32" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D33"/>
       <c r="E33" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F33" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="G33" t="n">
         <v>30</v>
@@ -1778,27 +2024,30 @@
         <v>99.7</v>
       </c>
       <c r="J33" t="s">
-        <v>92</v>
+        <v>122</v>
+      </c>
+      <c r="K33" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D34" t="n">
         <v>2760000</v>
       </c>
       <c r="E34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F34" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="G34" t="n">
         <v>29.82</v>
@@ -1810,27 +2059,30 @@
         <v>99.7</v>
       </c>
       <c r="J34" t="s">
-        <v>98</v>
+        <v>131</v>
+      </c>
+      <c r="K34" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D35" t="n">
         <v>123000</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F35" t="s">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="G35" t="n">
         <v>29.89</v>
@@ -1842,25 +2094,28 @@
         <v>99.8</v>
       </c>
       <c r="J35" t="s">
-        <v>101</v>
+        <v>135</v>
+      </c>
+      <c r="K35" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D36"/>
       <c r="E36" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F36" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="G36" t="n">
         <v>29.99</v>
@@ -1872,27 +2127,30 @@
         <v>99.9</v>
       </c>
       <c r="J36" t="s">
-        <v>98</v>
+        <v>131</v>
+      </c>
+      <c r="K36" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="C37" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D37" t="n">
         <v>51800</v>
       </c>
       <c r="E37" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F37" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="G37" t="n">
         <v>29.93</v>
@@ -1904,25 +2162,28 @@
         <v>99.8</v>
       </c>
       <c r="J37" t="s">
-        <v>98</v>
+        <v>131</v>
+      </c>
+      <c r="K37" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>143</v>
       </c>
       <c r="C38" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D38"/>
       <c r="E38" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F38" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
       <c r="G38" t="n">
         <v>29.82</v>
@@ -1934,25 +2195,28 @@
         <v>99.7</v>
       </c>
       <c r="J38" t="s">
-        <v>108</v>
+        <v>145</v>
+      </c>
+      <c r="K38" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="C39" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D39"/>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
       <c r="G39" t="n">
         <v>29.81</v>
@@ -1964,27 +2228,30 @@
         <v>99.6</v>
       </c>
       <c r="J39" t="s">
-        <v>108</v>
+        <v>145</v>
+      </c>
+      <c r="K39" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D40" t="n">
         <v>172000</v>
       </c>
       <c r="E40" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F40" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
       <c r="G40" t="n">
         <v>29.85</v>
@@ -1996,25 +2263,28 @@
         <v>99.8</v>
       </c>
       <c r="J40" t="s">
-        <v>108</v>
+        <v>145</v>
+      </c>
+      <c r="K40" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D41"/>
       <c r="E41" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F41" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="G41" t="n">
         <v>29.86</v>
@@ -2026,25 +2296,28 @@
         <v>99.8</v>
       </c>
       <c r="J41" t="s">
-        <v>115</v>
+        <v>155</v>
+      </c>
+      <c r="K41" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D42"/>
       <c r="E42" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="F42" t="s">
-        <v>118</v>
+        <v>159</v>
       </c>
       <c r="G42" t="n">
         <v>29.98</v>
@@ -2056,27 +2329,30 @@
         <v>99.8</v>
       </c>
       <c r="J42" t="s">
-        <v>119</v>
+        <v>160</v>
+      </c>
+      <c r="K42" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="B43" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D43" t="n">
         <v>166000</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F43" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="G43" t="n">
         <v>29.82</v>
@@ -2088,27 +2364,30 @@
         <v>99.8</v>
       </c>
       <c r="J43" t="s">
-        <v>123</v>
+        <v>165</v>
+      </c>
+      <c r="K43" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="B44" t="s">
-        <v>124</v>
+        <v>167</v>
       </c>
       <c r="C44" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D44" t="n">
         <v>16300</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F44" t="s">
-        <v>125</v>
+        <v>168</v>
       </c>
       <c r="G44" t="n">
         <v>29.83</v>
@@ -2120,25 +2399,28 @@
         <v>99.8</v>
       </c>
       <c r="J44" t="s">
-        <v>126</v>
+        <v>169</v>
+      </c>
+      <c r="K44" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="B45" t="s">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="C45" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D45"/>
       <c r="E45" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F45" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="G45" t="n">
         <v>29.84</v>
@@ -2150,27 +2432,30 @@
         <v>99.5</v>
       </c>
       <c r="J45" t="s">
-        <v>115</v>
+        <v>155</v>
+      </c>
+      <c r="K45" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>173</v>
       </c>
       <c r="B46" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="C46" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D46" t="n">
         <v>14500</v>
       </c>
       <c r="E46" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F46" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="G46" t="n">
         <v>29.41</v>
@@ -2182,25 +2467,28 @@
         <v>99.8</v>
       </c>
       <c r="J46" t="s">
-        <v>123</v>
+        <v>165</v>
+      </c>
+      <c r="K46" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>130</v>
+        <v>176</v>
       </c>
       <c r="B47" t="s">
-        <v>131</v>
+        <v>177</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D47"/>
       <c r="E47" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F47" t="s">
-        <v>132</v>
+        <v>178</v>
       </c>
       <c r="G47" t="n">
         <v>29.8</v>
@@ -2212,27 +2500,30 @@
         <v>99.8</v>
       </c>
       <c r="J47" t="s">
-        <v>133</v>
+        <v>179</v>
+      </c>
+      <c r="K47" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>176</v>
       </c>
       <c r="B48" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D48" t="n">
         <v>27900</v>
       </c>
       <c r="E48" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F48" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="G48" t="n">
         <v>29.91</v>
@@ -2244,25 +2535,28 @@
         <v>99.8</v>
       </c>
       <c r="J48" t="s">
-        <v>136</v>
+        <v>183</v>
+      </c>
+      <c r="K48" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>137</v>
+        <v>185</v>
       </c>
       <c r="B49" t="s">
-        <v>138</v>
+        <v>186</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D49"/>
       <c r="E49" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="F49" t="s">
-        <v>140</v>
+        <v>188</v>
       </c>
       <c r="G49" t="n">
         <v>27.21</v>
@@ -2274,25 +2568,28 @@
         <v>99.8</v>
       </c>
       <c r="J49" t="s">
-        <v>141</v>
+        <v>189</v>
+      </c>
+      <c r="K49" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>191</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>192</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D50"/>
       <c r="E50" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="F50" t="s">
-        <v>140</v>
+        <v>188</v>
       </c>
       <c r="G50" t="n">
         <v>30.02</v>
@@ -2304,7 +2601,10 @@
         <v>99.8</v>
       </c>
       <c r="J50" t="s">
-        <v>141</v>
+        <v>189</v>
+      </c>
+      <c r="K50" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a / b exp mergers
</commit_message>
<xml_diff>
--- a/summaries/longContigSampleSummary_gte90percentRef.xlsx
+++ b/summaries/longContigSampleSummary_gte90percentRef.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -50,97 +50,106 @@
     <t xml:space="preserve">197</t>
   </si>
   <si>
-    <t xml:space="preserve">VSP0009</t>
+    <t xml:space="preserve">VSP0009-1m</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> single experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3/30/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">197 ETA 20200330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0010</t>
   </si>
   <si>
     <t xml:space="preserve">composite</t>
   </si>
   <si>
-    <t xml:space="preserve">ETA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03/30/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">197 ETA 20200330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0010</t>
+    <t xml:space="preserve">4/8/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">203 ETA 20200408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">209 ETA 20200408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">210 ETA 20200408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0013-1m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4/13/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">211 ETA 20200413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">211-TCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0186-1m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/13/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">211-TCE ETA 20200413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0184-1m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP</t>
   </si>
   <si>
     <t xml:space="preserve">04/08/2020</t>
   </si>
   <si>
-    <t xml:space="preserve">20200408</t>
-  </si>
-  <si>
-    <t xml:space="preserve">203 ETA 20200408</t>
-  </si>
-  <si>
-    <t xml:space="preserve">209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">209 ETA 20200408</t>
-  </si>
-  <si>
-    <t xml:space="preserve">210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">210 ETA 20200408</t>
-  </si>
-  <si>
-    <t xml:space="preserve">211</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0186</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04/13/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200413</t>
-  </si>
-  <si>
-    <t xml:space="preserve">211 ET 20200413</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">211 ETA 20200413</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0184</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">211 NP 20200408</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0185</t>
+    <t xml:space="preserve">211-TCE NP 20200408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0185-1m</t>
   </si>
   <si>
     <t xml:space="preserve">OP</t>
   </si>
   <si>
-    <t xml:space="preserve">211 OP 20200413</t>
+    <t xml:space="preserve">211-TCE OP 20200413</t>
   </si>
   <si>
     <t xml:space="preserve">213</t>
@@ -149,7 +158,7 @@
     <t xml:space="preserve">VSP0014</t>
   </si>
   <si>
-    <t xml:space="preserve">04/15/2020</t>
+    <t xml:space="preserve">4/15/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200415</t>
@@ -158,10 +167,10 @@
     <t xml:space="preserve">213 ETA 20200415</t>
   </si>
   <si>
-    <t xml:space="preserve">222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0180</t>
+    <t xml:space="preserve">222-TCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0180-1m</t>
   </si>
   <si>
     <t xml:space="preserve">04/17/2020</t>
@@ -170,13 +179,13 @@
     <t xml:space="preserve">20200417</t>
   </si>
   <si>
-    <t xml:space="preserve">222 NP 20200417</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0181</t>
-  </si>
-  <si>
-    <t xml:space="preserve">222 OP 20200417</t>
+    <t xml:space="preserve">222-TCE NP 20200417</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0181-1m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">222-TCE OP 20200417</t>
   </si>
   <si>
     <t xml:space="preserve">VSP0182</t>
@@ -188,16 +197,16 @@
     <t xml:space="preserve">20200420</t>
   </si>
   <si>
-    <t xml:space="preserve">222 OP 20200420</t>
-  </si>
-  <si>
-    <t xml:space="preserve">223</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">223 OP 20200417</t>
+    <t xml:space="preserve">222-TCE OP 20200420</t>
+  </si>
+  <si>
+    <t xml:space="preserve">223-TCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0183-1m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">223-TCE OP 20200417</t>
   </si>
   <si>
     <t xml:space="preserve">227</t>
@@ -206,7 +215,7 @@
     <t xml:space="preserve">VSP0020</t>
   </si>
   <si>
-    <t xml:space="preserve">04/22/2020</t>
+    <t xml:space="preserve">4/22/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200422</t>
@@ -248,9 +257,6 @@
     <t xml:space="preserve">VSP0189-1</t>
   </si>
   <si>
-    <t xml:space="preserve"> single experiment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Saliva</t>
   </si>
   <si>
@@ -278,7 +284,7 @@
     <t xml:space="preserve">VSP0033</t>
   </si>
   <si>
-    <t xml:space="preserve">04/27/2020</t>
+    <t xml:space="preserve">4/27/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200427</t>
@@ -290,7 +296,7 @@
     <t xml:space="preserve">VSP0038</t>
   </si>
   <si>
-    <t xml:space="preserve">04/29/2020</t>
+    <t xml:space="preserve">4/29/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200429</t>
@@ -476,60 +482,69 @@
     <t xml:space="preserve">VSP0320-1</t>
   </si>
   <si>
+    <t xml:space="preserve">5/22/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">266 NP-OP 20200522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">266-TCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0262-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/20/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">266-TCE NP-OP 20200520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0263-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">266-TCE NP-OP 20200522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0176-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/27/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">269 ETA 20200527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0202-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/12/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">269 ETA 20200612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP0166-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">05/22/2020</t>
   </si>
   <si>
-    <t xml:space="preserve">20200522</t>
-  </si>
-  <si>
-    <t xml:space="preserve">266 NP-OP 20200522</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0262-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/20/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200520</t>
-  </si>
-  <si>
-    <t xml:space="preserve">266 Unk 20200520</t>
-  </si>
-  <si>
-    <t xml:space="preserve">269</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0176-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/27/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200527</t>
-  </si>
-  <si>
-    <t xml:space="preserve">269 ETA 20200527</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0202-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06/12/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200612</t>
-  </si>
-  <si>
-    <t xml:space="preserve">269 ETA 20200612</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP0166-1</t>
-  </si>
-  <si>
     <t xml:space="preserve">269 NP-OP 20200522</t>
   </si>
   <si>
@@ -572,13 +587,13 @@
     <t xml:space="preserve">CCLB</t>
   </si>
   <si>
-    <t xml:space="preserve">VSP0001</t>
+    <t xml:space="preserve">VSP0001-1m</t>
   </si>
   <si>
     <t xml:space="preserve">Vero cells</t>
   </si>
   <si>
-    <t xml:space="preserve">03/28/2020</t>
+    <t xml:space="preserve">3/28/2020</t>
   </si>
   <si>
     <t xml:space="preserve">20200328</t>
@@ -1001,14 +1016,14 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" t="n">
         <v>29.84</v>
@@ -1020,28 +1035,28 @@
         <v>99.4</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G4" t="n">
         <v>29.85</v>
@@ -1053,28 +1068,28 @@
         <v>99.4</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" t="n">
         <v>29.86</v>
@@ -1086,34 +1101,34 @@
         <v>99.7</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
         <v>32</v>
       </c>
       <c r="G6" t="n">
-        <v>29.8</v>
+        <v>29.9</v>
       </c>
       <c r="H6" t="n">
-        <v>99.9</v>
+        <v>99.8</v>
       </c>
       <c r="I6" t="n">
         <v>99.8</v>
@@ -1127,10 +1142,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
@@ -1140,13 +1155,13 @@
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G7" t="n">
-        <v>29.9</v>
+        <v>29.8</v>
       </c>
       <c r="H7" t="n">
-        <v>99.8</v>
+        <v>99.9</v>
       </c>
       <c r="I7" t="n">
         <v>99.8</v>
@@ -1155,25 +1170,25 @@
         <v>33</v>
       </c>
       <c r="K7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="G8" t="n">
         <v>29.86</v>
@@ -1185,28 +1200,28 @@
         <v>99.8</v>
       </c>
       <c r="J8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G9" t="n">
         <v>29.88</v>
@@ -1221,25 +1236,25 @@
         <v>33</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G10" t="n">
         <v>29.86</v>
@@ -1251,28 +1266,28 @@
         <v>99.7</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="K10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G11" t="n">
         <v>29.87</v>
@@ -1284,31 +1299,31 @@
         <v>99.7</v>
       </c>
       <c r="J11" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="K11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G12" t="n">
-        <v>29.34</v>
+        <v>30.04</v>
       </c>
       <c r="H12" t="n">
         <v>99.9</v>
@@ -1317,28 +1332,28 @@
         <v>99.9</v>
       </c>
       <c r="J12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="K12" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G13" t="n">
         <v>29.88</v>
@@ -1350,28 +1365,28 @@
         <v>99.9</v>
       </c>
       <c r="J13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K13" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G14" t="n">
         <v>29.96</v>
@@ -1383,28 +1398,28 @@
         <v>99.9</v>
       </c>
       <c r="J14" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="K14" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G15" t="n">
         <v>29.91</v>
@@ -1416,28 +1431,28 @@
         <v>99.8</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G16" t="n">
         <v>29.82</v>
@@ -1449,28 +1464,28 @@
         <v>99.8</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F17" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G17" t="n">
         <v>29.9</v>
@@ -1482,28 +1497,28 @@
         <v>99.8</v>
       </c>
       <c r="J17" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="K17" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G18" t="n">
         <v>29.68</v>
@@ -1515,30 +1530,30 @@
         <v>98.8</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D19" t="n">
         <v>85100</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G19" t="n">
         <v>29.82</v>
@@ -1550,30 +1565,30 @@
         <v>99.8</v>
       </c>
       <c r="J19" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="K19" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D20" t="n">
         <v>176000</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G20" t="n">
         <v>29.87</v>
@@ -1585,28 +1600,28 @@
         <v>99.8</v>
       </c>
       <c r="J20" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K20" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G21" t="n">
         <v>29.97</v>
@@ -1618,28 +1633,28 @@
         <v>99.8</v>
       </c>
       <c r="J21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K21" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G22" t="n">
         <v>29.92</v>
@@ -1651,28 +1666,28 @@
         <v>99.5</v>
       </c>
       <c r="J22" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K22" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G23" t="n">
         <v>29.89</v>
@@ -1684,28 +1699,28 @@
         <v>99.8</v>
       </c>
       <c r="J23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G24" t="n">
         <v>30.06</v>
@@ -1717,28 +1732,28 @@
         <v>99.8</v>
       </c>
       <c r="J24" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K24" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G25" t="n">
         <v>27.48</v>
@@ -1750,30 +1765,30 @@
         <v>99.8</v>
       </c>
       <c r="J25" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K25" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D26" t="n">
         <v>364000</v>
       </c>
       <c r="E26" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F26" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G26" t="n">
         <v>29.45</v>
@@ -1785,21 +1800,21 @@
         <v>99.8</v>
       </c>
       <c r="J26" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K26" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D27" t="n">
         <v>1420000</v>
@@ -1808,7 +1823,7 @@
         <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G27" t="n">
         <v>29.31</v>
@@ -1820,28 +1835,28 @@
         <v>99.7</v>
       </c>
       <c r="J27" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K27" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F28" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G28" t="n">
         <v>29.88</v>
@@ -1853,30 +1868,30 @@
         <v>99.8</v>
       </c>
       <c r="J28" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K28" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D29" t="n">
         <v>222000</v>
       </c>
       <c r="E29" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F29" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G29" t="n">
         <v>29.89</v>
@@ -1888,30 +1903,30 @@
         <v>99.8</v>
       </c>
       <c r="J29" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K29" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D30" t="n">
         <v>667</v>
       </c>
       <c r="E30" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F30" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G30" t="n">
         <v>29.72</v>
@@ -1923,21 +1938,21 @@
         <v>99.2</v>
       </c>
       <c r="J30" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K30" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D31" t="n">
         <v>255500</v>
@@ -1946,7 +1961,7 @@
         <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G31" t="n">
         <v>29.82</v>
@@ -1958,28 +1973,28 @@
         <v>99.8</v>
       </c>
       <c r="J31" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K31" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B32" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D32"/>
       <c r="E32" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F32" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G32" t="n">
         <v>29.94</v>
@@ -1991,28 +2006,28 @@
         <v>99.8</v>
       </c>
       <c r="J32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K32" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D33"/>
       <c r="E33" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F33" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G33" t="n">
         <v>30</v>
@@ -2024,21 +2039,21 @@
         <v>99.7</v>
       </c>
       <c r="J33" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K33" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D34" t="n">
         <v>2760000</v>
@@ -2047,7 +2062,7 @@
         <v>14</v>
       </c>
       <c r="F34" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G34" t="n">
         <v>29.82</v>
@@ -2059,21 +2074,21 @@
         <v>99.7</v>
       </c>
       <c r="J34" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K34" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B35" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D35" t="n">
         <v>123000</v>
@@ -2082,7 +2097,7 @@
         <v>14</v>
       </c>
       <c r="F35" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G35" t="n">
         <v>29.89</v>
@@ -2094,28 +2109,28 @@
         <v>99.8</v>
       </c>
       <c r="J35" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K35" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D36"/>
       <c r="E36" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F36" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G36" t="n">
         <v>29.99</v>
@@ -2127,30 +2142,30 @@
         <v>99.9</v>
       </c>
       <c r="J36" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K36" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D37" t="n">
         <v>51800</v>
       </c>
       <c r="E37" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F37" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G37" t="n">
         <v>29.93</v>
@@ -2162,28 +2177,28 @@
         <v>99.8</v>
       </c>
       <c r="J37" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K37" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B38" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D38"/>
       <c r="E38" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F38" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G38" t="n">
         <v>29.82</v>
@@ -2195,28 +2210,28 @@
         <v>99.7</v>
       </c>
       <c r="J38" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K38" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B39" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D39"/>
       <c r="E39" t="s">
         <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G39" t="n">
         <v>29.81</v>
@@ -2228,30 +2243,30 @@
         <v>99.6</v>
       </c>
       <c r="J39" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K39" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B40" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C40" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D40" t="n">
         <v>172000</v>
       </c>
       <c r="E40" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F40" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G40" t="n">
         <v>29.85</v>
@@ -2263,28 +2278,28 @@
         <v>99.8</v>
       </c>
       <c r="J40" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K40" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B41" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D41"/>
       <c r="E41" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F41" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G41" t="n">
         <v>29.86</v>
@@ -2296,28 +2311,28 @@
         <v>99.8</v>
       </c>
       <c r="J41" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="K41" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B42" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D42"/>
       <c r="E42" t="s">
-        <v>158</v>
+        <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="G42" t="n">
         <v>29.98</v>
@@ -2329,59 +2344,57 @@
         <v>99.8</v>
       </c>
       <c r="J42" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="K42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B43" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
-      </c>
-      <c r="D43" t="n">
-        <v>166000</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D43"/>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="F43" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="G43" t="n">
-        <v>29.82</v>
+        <v>29.86</v>
       </c>
       <c r="H43" t="n">
-        <v>99.8</v>
+        <v>99.9</v>
       </c>
       <c r="I43" t="n">
-        <v>99.8</v>
+        <v>99.6</v>
       </c>
       <c r="J43" t="s">
+        <v>157</v>
+      </c>
+      <c r="K43" t="s">
         <v>165</v>
-      </c>
-      <c r="K43" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B44" t="s">
         <v>167</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="D44" t="n">
-        <v>16300</v>
+        <v>166000</v>
       </c>
       <c r="E44" t="s">
         <v>14</v>
@@ -2390,7 +2403,7 @@
         <v>168</v>
       </c>
       <c r="G44" t="n">
-        <v>29.83</v>
+        <v>29.82</v>
       </c>
       <c r="H44" t="n">
         <v>99.8</v>
@@ -2407,91 +2420,93 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B45" t="s">
         <v>171</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
-      </c>
-      <c r="D45"/>
+        <v>13</v>
+      </c>
+      <c r="D45" t="n">
+        <v>16300</v>
+      </c>
       <c r="E45" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="F45" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="G45" t="n">
-        <v>29.84</v>
+        <v>29.83</v>
       </c>
       <c r="H45" t="n">
         <v>99.8</v>
       </c>
       <c r="I45" t="n">
-        <v>99.5</v>
+        <v>99.8</v>
       </c>
       <c r="J45" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="K45" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B46" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46" t="n">
-        <v>14500</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D46"/>
       <c r="E46" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F46" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="G46" t="n">
-        <v>29.41</v>
+        <v>29.84</v>
       </c>
       <c r="H46" t="n">
         <v>99.8</v>
       </c>
       <c r="I46" t="n">
-        <v>99.8</v>
+        <v>99.5</v>
       </c>
       <c r="J46" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="K46" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B47" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C47" t="s">
         <v>13</v>
       </c>
-      <c r="D47"/>
+      <c r="D47" t="n">
+        <v>14500</v>
+      </c>
       <c r="E47" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F47" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="G47" t="n">
-        <v>29.8</v>
+        <v>29.41</v>
       </c>
       <c r="H47" t="n">
         <v>99.8</v>
@@ -2500,7 +2515,7 @@
         <v>99.8</v>
       </c>
       <c r="J47" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="K47" t="s">
         <v>180</v>
@@ -2508,25 +2523,23 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B48" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
-      </c>
-      <c r="D48" t="n">
-        <v>27900</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D48"/>
       <c r="E48" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F48" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G48" t="n">
-        <v>29.91</v>
+        <v>29.8</v>
       </c>
       <c r="H48" t="n">
         <v>99.8</v>
@@ -2535,15 +2548,15 @@
         <v>99.8</v>
       </c>
       <c r="J48" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K48" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B49" t="s">
         <v>186</v>
@@ -2551,60 +2564,95 @@
       <c r="C49" t="s">
         <v>13</v>
       </c>
-      <c r="D49"/>
+      <c r="D49" t="n">
+        <v>27900</v>
+      </c>
       <c r="E49" t="s">
+        <v>74</v>
+      </c>
+      <c r="F49" t="s">
         <v>187</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="n">
+        <v>29.91</v>
+      </c>
+      <c r="H49" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="I49" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="J49" t="s">
         <v>188</v>
       </c>
-      <c r="G49" t="n">
-        <v>27.21</v>
-      </c>
-      <c r="H49" t="n">
-        <v>99.9</v>
-      </c>
-      <c r="I49" t="n">
-        <v>99.8</v>
-      </c>
-      <c r="J49" t="s">
+      <c r="K49" t="s">
         <v>189</v>
-      </c>
-      <c r="K49" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>190</v>
+      </c>
+      <c r="B50" t="s">
         <v>191</v>
-      </c>
-      <c r="B50" t="s">
-        <v>192</v>
       </c>
       <c r="C50" t="s">
         <v>13</v>
       </c>
       <c r="D50"/>
       <c r="E50" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="F50" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G50" t="n">
+        <v>27.21</v>
+      </c>
+      <c r="H50" t="n">
+        <v>99.9</v>
+      </c>
+      <c r="I50" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="J50" t="s">
+        <v>194</v>
+      </c>
+      <c r="K50" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51" t="s">
+        <v>197</v>
+      </c>
+      <c r="C51" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51"/>
+      <c r="E51" t="s">
+        <v>192</v>
+      </c>
+      <c r="F51" t="s">
+        <v>193</v>
+      </c>
+      <c r="G51" t="n">
         <v>30.02</v>
       </c>
-      <c r="H50" t="n">
-        <v>99.8</v>
-      </c>
-      <c r="I50" t="n">
-        <v>99.8</v>
-      </c>
-      <c r="J50" t="s">
-        <v>189</v>
-      </c>
-      <c r="K50" t="s">
-        <v>193</v>
+      <c r="H51" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="I51" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="J51" t="s">
+        <v>194</v>
+      </c>
+      <c r="K51" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added patient meta data, collapsed dup genomes
</commit_message>
<xml_diff>
--- a/summaries/longContigSampleSummary_gte90percentRef.xlsx
+++ b/summaries/longContigSampleSummary_gte90percentRef.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">ETA</t>
   </si>
   <si>
-    <t xml:space="preserve">3/30/2020</t>
+    <t xml:space="preserve">2020-03-30</t>
   </si>
   <si>
     <t xml:space="preserve">20200330</t>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">composite</t>
   </si>
   <si>
-    <t xml:space="preserve">4/8/2020</t>
+    <t xml:space="preserve">2020-04-08</t>
   </si>
   <si>
     <t xml:space="preserve">20200408</t>
@@ -110,7 +110,7 @@
     <t xml:space="preserve">VSP0013-1m</t>
   </si>
   <si>
-    <t xml:space="preserve">4/13/2020</t>
+    <t xml:space="preserve">2020-04-13</t>
   </si>
   <si>
     <t xml:space="preserve">20200413</t>
@@ -125,9 +125,6 @@
     <t xml:space="preserve">VSP0186-1m</t>
   </si>
   <si>
-    <t xml:space="preserve">04/13/2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">211-TCE ETA 20200413</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t xml:space="preserve">NP</t>
   </si>
   <si>
-    <t xml:space="preserve">04/08/2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">211-TCE NP 20200408</t>
   </si>
   <si>
@@ -158,7 +152,7 @@
     <t xml:space="preserve">VSP0014</t>
   </si>
   <si>
-    <t xml:space="preserve">4/15/2020</t>
+    <t xml:space="preserve">2020-04-15</t>
   </si>
   <si>
     <t xml:space="preserve">20200415</t>
@@ -173,7 +167,7 @@
     <t xml:space="preserve">VSP0180-1m</t>
   </si>
   <si>
-    <t xml:space="preserve">04/17/2020</t>
+    <t xml:space="preserve">2020-04-17</t>
   </si>
   <si>
     <t xml:space="preserve">20200417</t>
@@ -191,7 +185,7 @@
     <t xml:space="preserve">VSP0182</t>
   </si>
   <si>
-    <t xml:space="preserve">04/20/2020</t>
+    <t xml:space="preserve">2020-04-20</t>
   </si>
   <si>
     <t xml:space="preserve">20200420</t>
@@ -215,7 +209,7 @@
     <t xml:space="preserve">VSP0020</t>
   </si>
   <si>
-    <t xml:space="preserve">4/22/2020</t>
+    <t xml:space="preserve">2020-04-22</t>
   </si>
   <si>
     <t xml:space="preserve">20200422</t>
@@ -239,7 +233,7 @@
     <t xml:space="preserve">NP-OP</t>
   </si>
   <si>
-    <t xml:space="preserve">05/29/2020</t>
+    <t xml:space="preserve">2020-05-29</t>
   </si>
   <si>
     <t xml:space="preserve">20200529</t>
@@ -269,7 +263,7 @@
     <t xml:space="preserve">VSP0080-1</t>
   </si>
   <si>
-    <t xml:space="preserve">04/24/2020</t>
+    <t xml:space="preserve">2020-04-24</t>
   </si>
   <si>
     <t xml:space="preserve">20200424</t>
@@ -284,7 +278,7 @@
     <t xml:space="preserve">VSP0033</t>
   </si>
   <si>
-    <t xml:space="preserve">4/27/2020</t>
+    <t xml:space="preserve">2020-04-27</t>
   </si>
   <si>
     <t xml:space="preserve">20200427</t>
@@ -296,7 +290,7 @@
     <t xml:space="preserve">VSP0038</t>
   </si>
   <si>
-    <t xml:space="preserve">4/29/2020</t>
+    <t xml:space="preserve">2020-04-29</t>
   </si>
   <si>
     <t xml:space="preserve">20200429</t>
@@ -335,7 +329,7 @@
     <t xml:space="preserve">VSP0046-1</t>
   </si>
   <si>
-    <t xml:space="preserve">05/01/2020</t>
+    <t xml:space="preserve">2020-05-01</t>
   </si>
   <si>
     <t xml:space="preserve">20200501</t>
@@ -350,7 +344,7 @@
     <t xml:space="preserve">VSP0052-1</t>
   </si>
   <si>
-    <t xml:space="preserve">05/04/2020</t>
+    <t xml:space="preserve">2020-05-04</t>
   </si>
   <si>
     <t xml:space="preserve">20200504</t>
@@ -383,7 +377,7 @@
     <t xml:space="preserve">VSP0088-1</t>
   </si>
   <si>
-    <t xml:space="preserve">05/06/2020</t>
+    <t xml:space="preserve">2020-05-06</t>
   </si>
   <si>
     <t xml:space="preserve">20200506</t>
@@ -410,7 +404,7 @@
     <t xml:space="preserve">VSP0100-1</t>
   </si>
   <si>
-    <t xml:space="preserve">05/08/2020</t>
+    <t xml:space="preserve">2020-05-08</t>
   </si>
   <si>
     <t xml:space="preserve">20200508</t>
@@ -422,7 +416,7 @@
     <t xml:space="preserve">VSP0123-1</t>
   </si>
   <si>
-    <t xml:space="preserve">05/11/2020</t>
+    <t xml:space="preserve">2020-05-11</t>
   </si>
   <si>
     <t xml:space="preserve">20200511</t>
@@ -452,7 +446,7 @@
     <t xml:space="preserve">VSP0141-1</t>
   </si>
   <si>
-    <t xml:space="preserve">05/15/2020</t>
+    <t xml:space="preserve">2020-05-15</t>
   </si>
   <si>
     <t xml:space="preserve">20200515</t>
@@ -482,7 +476,7 @@
     <t xml:space="preserve">VSP0320-1</t>
   </si>
   <si>
-    <t xml:space="preserve">5/22/20</t>
+    <t xml:space="preserve">2020-05-22</t>
   </si>
   <si>
     <t xml:space="preserve">20200522</t>
@@ -497,7 +491,7 @@
     <t xml:space="preserve">VSP0262-1</t>
   </si>
   <si>
-    <t xml:space="preserve">5/20/20</t>
+    <t xml:space="preserve">2020-05-20</t>
   </si>
   <si>
     <t xml:space="preserve">20200520</t>
@@ -518,7 +512,7 @@
     <t xml:space="preserve">VSP0176-1</t>
   </si>
   <si>
-    <t xml:space="preserve">05/27/2020</t>
+    <t xml:space="preserve">2020-05-27</t>
   </si>
   <si>
     <t xml:space="preserve">20200527</t>
@@ -530,7 +524,7 @@
     <t xml:space="preserve">VSP0202-1</t>
   </si>
   <si>
-    <t xml:space="preserve">06/12/2020</t>
+    <t xml:space="preserve">2020-06-12</t>
   </si>
   <si>
     <t xml:space="preserve">20200612</t>
@@ -542,9 +536,6 @@
     <t xml:space="preserve">VSP0166-1</t>
   </si>
   <si>
-    <t xml:space="preserve">05/22/2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">269 NP-OP 20200522</t>
   </si>
   <si>
@@ -563,7 +554,7 @@
     <t xml:space="preserve">VSP0230</t>
   </si>
   <si>
-    <t xml:space="preserve">06/29/2020</t>
+    <t xml:space="preserve">2020-06-29</t>
   </si>
   <si>
     <t xml:space="preserve">20200629</t>
@@ -575,7 +566,7 @@
     <t xml:space="preserve">VSP0233-2</t>
   </si>
   <si>
-    <t xml:space="preserve">07/01/2020</t>
+    <t xml:space="preserve">2020-07-01</t>
   </si>
   <si>
     <t xml:space="preserve">20200701</t>
@@ -593,7 +584,7 @@
     <t xml:space="preserve">Vero cells</t>
   </si>
   <si>
-    <t xml:space="preserve">3/28/2020</t>
+    <t xml:space="preserve">2020-03-28</t>
   </si>
   <si>
     <t xml:space="preserve">20200328</t>
@@ -1155,7 +1146,7 @@
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G7" t="n">
         <v>29.8</v>
@@ -1170,7 +1161,7 @@
         <v>33</v>
       </c>
       <c r="K7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
@@ -1178,17 +1169,17 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="G8" t="n">
         <v>29.86</v>
@@ -1203,7 +1194,7 @@
         <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
@@ -1211,17 +1202,17 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G9" t="n">
         <v>29.88</v>
@@ -1236,15 +1227,15 @@
         <v>33</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -1254,7 +1245,7 @@
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G10" t="n">
         <v>29.86</v>
@@ -1266,28 +1257,28 @@
         <v>99.7</v>
       </c>
       <c r="J10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G11" t="n">
         <v>29.87</v>
@@ -1299,28 +1290,28 @@
         <v>99.7</v>
       </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G12" t="n">
         <v>30.04</v>
@@ -1332,28 +1323,28 @@
         <v>99.9</v>
       </c>
       <c r="J12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G13" t="n">
         <v>29.88</v>
@@ -1365,28 +1356,28 @@
         <v>99.9</v>
       </c>
       <c r="J13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G14" t="n">
         <v>29.96</v>
@@ -1398,28 +1389,28 @@
         <v>99.9</v>
       </c>
       <c r="J14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G15" t="n">
         <v>29.91</v>
@@ -1431,28 +1422,28 @@
         <v>99.8</v>
       </c>
       <c r="J15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G16" t="n">
         <v>29.82</v>
@@ -1464,28 +1455,28 @@
         <v>99.8</v>
       </c>
       <c r="J16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G17" t="n">
         <v>29.9</v>
@@ -1497,28 +1488,28 @@
         <v>99.8</v>
       </c>
       <c r="J17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G18" t="n">
         <v>29.68</v>
@@ -1530,18 +1521,18 @@
         <v>98.8</v>
       </c>
       <c r="J18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
         <v>13</v>
@@ -1550,10 +1541,10 @@
         <v>85100</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G19" t="n">
         <v>29.82</v>
@@ -1565,18 +1556,18 @@
         <v>99.8</v>
       </c>
       <c r="J19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
         <v>13</v>
@@ -1585,10 +1576,10 @@
         <v>176000</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G20" t="n">
         <v>29.87</v>
@@ -1600,28 +1591,28 @@
         <v>99.8</v>
       </c>
       <c r="J20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G21" t="n">
         <v>29.97</v>
@@ -1633,28 +1624,28 @@
         <v>99.8</v>
       </c>
       <c r="J21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G22" t="n">
         <v>29.92</v>
@@ -1666,28 +1657,28 @@
         <v>99.5</v>
       </c>
       <c r="J22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G23" t="n">
         <v>29.89</v>
@@ -1699,28 +1690,28 @@
         <v>99.8</v>
       </c>
       <c r="J23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G24" t="n">
         <v>30.06</v>
@@ -1732,28 +1723,28 @@
         <v>99.8</v>
       </c>
       <c r="J24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
         <v>20</v>
       </c>
       <c r="D25"/>
       <c r="E25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G25" t="n">
         <v>27.48</v>
@@ -1765,18 +1756,18 @@
         <v>99.8</v>
       </c>
       <c r="J25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C26" t="s">
         <v>13</v>
@@ -1785,10 +1776,10 @@
         <v>364000</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G26" t="n">
         <v>29.45</v>
@@ -1800,18 +1791,18 @@
         <v>99.8</v>
       </c>
       <c r="J26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
         <v>13</v>
@@ -1823,7 +1814,7 @@
         <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G27" t="n">
         <v>29.31</v>
@@ -1835,28 +1826,28 @@
         <v>99.7</v>
       </c>
       <c r="J27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G28" t="n">
         <v>29.88</v>
@@ -1868,18 +1859,18 @@
         <v>99.8</v>
       </c>
       <c r="J28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C29" t="s">
         <v>13</v>
@@ -1888,10 +1879,10 @@
         <v>222000</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G29" t="n">
         <v>29.89</v>
@@ -1903,18 +1894,18 @@
         <v>99.8</v>
       </c>
       <c r="J29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
         <v>13</v>
@@ -1923,10 +1914,10 @@
         <v>667</v>
       </c>
       <c r="E30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G30" t="n">
         <v>29.72</v>
@@ -1938,18 +1929,18 @@
         <v>99.2</v>
       </c>
       <c r="J30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
         <v>13</v>
@@ -1961,7 +1952,7 @@
         <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G31" t="n">
         <v>29.82</v>
@@ -1973,28 +1964,28 @@
         <v>99.8</v>
       </c>
       <c r="J31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
       </c>
       <c r="D32"/>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G32" t="n">
         <v>29.94</v>
@@ -2006,28 +1997,28 @@
         <v>99.8</v>
       </c>
       <c r="J32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K32" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
         <v>20</v>
       </c>
       <c r="D33"/>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G33" t="n">
         <v>30</v>
@@ -2039,18 +2030,18 @@
         <v>99.7</v>
       </c>
       <c r="J33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
@@ -2062,7 +2053,7 @@
         <v>14</v>
       </c>
       <c r="F34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G34" t="n">
         <v>29.82</v>
@@ -2074,18 +2065,18 @@
         <v>99.7</v>
       </c>
       <c r="J34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C35" t="s">
         <v>13</v>
@@ -2097,7 +2088,7 @@
         <v>14</v>
       </c>
       <c r="F35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G35" t="n">
         <v>29.89</v>
@@ -2109,28 +2100,28 @@
         <v>99.8</v>
       </c>
       <c r="J35" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B36" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
         <v>20</v>
       </c>
       <c r="D36"/>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G36" t="n">
         <v>29.99</v>
@@ -2142,18 +2133,18 @@
         <v>99.9</v>
       </c>
       <c r="J36" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C37" t="s">
         <v>13</v>
@@ -2162,10 +2153,10 @@
         <v>51800</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G37" t="n">
         <v>29.93</v>
@@ -2177,28 +2168,28 @@
         <v>99.8</v>
       </c>
       <c r="J37" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
       </c>
       <c r="D38"/>
       <c r="E38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G38" t="n">
         <v>29.82</v>
@@ -2210,18 +2201,18 @@
         <v>99.7</v>
       </c>
       <c r="J38" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C39" t="s">
         <v>13</v>
@@ -2231,7 +2222,7 @@
         <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G39" t="n">
         <v>29.81</v>
@@ -2243,18 +2234,18 @@
         <v>99.6</v>
       </c>
       <c r="J39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K39" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C40" t="s">
         <v>13</v>
@@ -2263,10 +2254,10 @@
         <v>172000</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F40" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G40" t="n">
         <v>29.85</v>
@@ -2278,28 +2269,30 @@
         <v>99.8</v>
       </c>
       <c r="J40" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" t="n">
+        <v>5750000</v>
+      </c>
+      <c r="E41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F41" t="s">
         <v>154</v>
-      </c>
-      <c r="B41" t="s">
-        <v>155</v>
-      </c>
-      <c r="C41" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41"/>
-      <c r="E41" t="s">
-        <v>74</v>
-      </c>
-      <c r="F41" t="s">
-        <v>156</v>
       </c>
       <c r="G41" t="n">
         <v>29.86</v>
@@ -2311,28 +2304,30 @@
         <v>99.8</v>
       </c>
       <c r="J41" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>157</v>
+      </c>
+      <c r="B42" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" t="n">
+        <v>58500000000</v>
+      </c>
+      <c r="E42" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" t="s">
         <v>159</v>
-      </c>
-      <c r="B42" t="s">
-        <v>160</v>
-      </c>
-      <c r="C42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42"/>
-      <c r="E42" t="s">
-        <v>74</v>
-      </c>
-      <c r="F42" t="s">
-        <v>161</v>
       </c>
       <c r="G42" t="n">
         <v>29.98</v>
@@ -2344,28 +2339,30 @@
         <v>99.8</v>
       </c>
       <c r="J42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K42" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B43" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C43" t="s">
         <v>13</v>
       </c>
-      <c r="D43"/>
+      <c r="D43" t="n">
+        <v>37550000000</v>
+      </c>
       <c r="E43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G43" t="n">
         <v>29.86</v>
@@ -2377,18 +2374,18 @@
         <v>99.6</v>
       </c>
       <c r="J43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K43" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B44" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C44" t="s">
         <v>13</v>
@@ -2400,7 +2397,7 @@
         <v>14</v>
       </c>
       <c r="F44" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G44" t="n">
         <v>29.82</v>
@@ -2412,18 +2409,18 @@
         <v>99.8</v>
       </c>
       <c r="J44" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C45" t="s">
         <v>13</v>
@@ -2435,7 +2432,7 @@
         <v>14</v>
       </c>
       <c r="F45" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G45" t="n">
         <v>29.83</v>
@@ -2447,28 +2444,28 @@
         <v>99.8</v>
       </c>
       <c r="J45" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K45" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C46" t="s">
         <v>13</v>
       </c>
       <c r="D46"/>
       <c r="E46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F46" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="G46" t="n">
         <v>29.84</v>
@@ -2480,18 +2477,18 @@
         <v>99.5</v>
       </c>
       <c r="J46" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K46" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B47" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C47" t="s">
         <v>13</v>
@@ -2500,10 +2497,10 @@
         <v>14500</v>
       </c>
       <c r="E47" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F47" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G47" t="n">
         <v>29.41</v>
@@ -2515,28 +2512,28 @@
         <v>99.8</v>
       </c>
       <c r="J47" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K47" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B48" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C48" t="s">
         <v>20</v>
       </c>
       <c r="D48"/>
       <c r="E48" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F48" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G48" t="n">
         <v>29.8</v>
@@ -2548,18 +2545,18 @@
         <v>99.8</v>
       </c>
       <c r="J48" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K48" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B49" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C49" t="s">
         <v>13</v>
@@ -2568,10 +2565,10 @@
         <v>27900</v>
       </c>
       <c r="E49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F49" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G49" t="n">
         <v>29.91</v>
@@ -2583,28 +2580,28 @@
         <v>99.8</v>
       </c>
       <c r="J49" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K49" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B50" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C50" t="s">
         <v>13</v>
       </c>
       <c r="D50"/>
       <c r="E50" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F50" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G50" t="n">
         <v>27.21</v>
@@ -2616,28 +2613,28 @@
         <v>99.8</v>
       </c>
       <c r="J50" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K50" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B51" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C51" t="s">
         <v>20</v>
       </c>
       <c r="D51"/>
       <c r="E51" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F51" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G51" t="n">
         <v>30.02</v>
@@ -2649,10 +2646,10 @@
         <v>99.8</v>
       </c>
       <c r="J51" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K51" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
De Wit sample data
</commit_message>
<xml_diff>
--- a/summaries/longContigSampleSummary_gte90percentRef.xlsx
+++ b/summaries/longContigSampleSummary_gte90percentRef.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -47,160 +47,166 @@
     <t xml:space="preserve">sampleName</t>
   </si>
   <si>
-    <t xml:space="preserve">SRR11783571</t>
+    <t xml:space="preserve">deWit_RM2_Remdesivir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8013-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> single experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nose_swab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-06-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM2_Remdesivir Nose_swab 20200606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM3_Remdesivir</t>
   </si>
   <si>
     <t xml:space="preserve">VSP8024-1</t>
   </si>
   <si>
-    <t xml:space="preserve"> single experiment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020-09-29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783571 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783573</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8013-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783573 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783592</t>
+    <t xml:space="preserve">BAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-06-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM3_Remdesivir BAL 20200604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8031-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM3_Remdesivir Nose_swab 20200606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8011-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RLLL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-06-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM3_Remdesivir RLLL 20200608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM4_Remdesivir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8045-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM4_Remdesivir BAL 20200604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8005-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM4_Remdesivir Nose_swab 20200606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM5_Remdesivir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8021-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM5_Remdesivir BAL 20200604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM6_Remdesivir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8009-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM6_Remdesivir BAL 20200604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM7_Vehicle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8036-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM7_Vehicle BAL 20200604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8015-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rectal_swab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-06-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20200603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM7_Vehicle Rectal_swab 20200603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8035-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM7_Vehicle RLLL 20200608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM8_Vehicle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8041-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM8_Vehicle BAL 20200604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8034-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLLL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM8_Vehicle LLLL 20200608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8029-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM8_Vehicle Rectal_swab 20200603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM9_Vehicle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSP8007-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deWit_RM9_Vehicle BAL 20200604</t>
   </si>
   <si>
     <t xml:space="preserve">VSP8014-1</t>
   </si>
   <si>
-    <t xml:space="preserve">SRR11783592 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783594</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8007-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783594 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783595</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8029-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783595 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783598</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8034-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783598 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783599</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8041-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783599 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8015-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783600 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783601</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8035-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783601 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783605</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8036-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783605 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783610</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8009-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783610 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783615</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8021-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783615 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783618</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8005-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783618 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783620</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8045-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783620 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783622</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8011-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783622 Unk 20200929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783623</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSP8031-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRR11783623 Unk 20200929</t>
+    <t xml:space="preserve">deWit_RM9_Vehicle Nose_swab 20200606</t>
   </si>
 </sst>
 </file>
@@ -585,7 +591,7 @@
         <v>15</v>
       </c>
       <c r="G2" t="n">
-        <v>29.94</v>
+        <v>29.96</v>
       </c>
       <c r="H2" t="n">
         <v>100</v>
@@ -612,13 +618,13 @@
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G3" t="n">
-        <v>29.96</v>
+        <v>29.94</v>
       </c>
       <c r="H3" t="n">
         <v>100</v>
@@ -627,18 +633,18 @@
         <v>100</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -651,7 +657,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="n">
-        <v>30.01</v>
+        <v>29.97</v>
       </c>
       <c r="H4" t="n">
         <v>100</v>
@@ -663,25 +669,25 @@
         <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G5" t="n">
         <v>30.09</v>
@@ -693,51 +699,51 @@
         <v>100</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G6" t="n">
-        <v>29.96</v>
+        <v>29.98</v>
       </c>
       <c r="H6" t="n">
-        <v>100</v>
+        <v>99.9</v>
       </c>
       <c r="I6" t="n">
-        <v>100</v>
+        <v>99.9</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
@@ -750,7 +756,7 @@
         <v>15</v>
       </c>
       <c r="G7" t="n">
-        <v>30.09</v>
+        <v>30.1</v>
       </c>
       <c r="H7" t="n">
         <v>100</v>
@@ -762,28 +768,28 @@
         <v>16</v>
       </c>
       <c r="K7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G8" t="n">
-        <v>30.11</v>
+        <v>29.86</v>
       </c>
       <c r="H8" t="n">
         <v>100</v>
@@ -792,64 +798,64 @@
         <v>100</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G9" t="n">
-        <v>29.98</v>
+        <v>30</v>
       </c>
       <c r="H9" t="n">
         <v>100</v>
       </c>
       <c r="I9" t="n">
-        <v>99.9</v>
+        <v>100</v>
       </c>
       <c r="J9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G10" t="n">
-        <v>29.84</v>
+        <v>29.87</v>
       </c>
       <c r="H10" t="n">
         <v>100</v>
@@ -858,10 +864,10 @@
         <v>100</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11">
@@ -869,53 +875,53 @@
         <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="G11" t="n">
-        <v>29.87</v>
+        <v>29.98</v>
       </c>
       <c r="H11" t="n">
         <v>100</v>
       </c>
       <c r="I11" t="n">
-        <v>100</v>
+        <v>99.9</v>
       </c>
       <c r="J11" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="K11" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G12" t="n">
-        <v>30</v>
+        <v>29.84</v>
       </c>
       <c r="H12" t="n">
         <v>100</v>
@@ -924,31 +930,31 @@
         <v>100</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="K12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G13" t="n">
-        <v>29.86</v>
+        <v>30.11</v>
       </c>
       <c r="H13" t="n">
         <v>100</v>
@@ -957,31 +963,31 @@
         <v>100</v>
       </c>
       <c r="J13" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G14" t="n">
-        <v>30.1</v>
+        <v>30.09</v>
       </c>
       <c r="H14" t="n">
         <v>100</v>
@@ -990,61 +996,61 @@
         <v>100</v>
       </c>
       <c r="J14" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="K14" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="G15" t="n">
-        <v>29.98</v>
+        <v>29.96</v>
       </c>
       <c r="H15" t="n">
-        <v>99.9</v>
+        <v>100</v>
       </c>
       <c r="I15" t="n">
-        <v>99.9</v>
+        <v>100</v>
       </c>
       <c r="J15" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="K15" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G16" t="n">
         <v>30.09</v>
@@ -1056,10 +1062,10 @@
         <v>100</v>
       </c>
       <c r="J16" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="K16" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17">
@@ -1067,7 +1073,7 @@
         <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -1080,7 +1086,7 @@
         <v>15</v>
       </c>
       <c r="G17" t="n">
-        <v>29.97</v>
+        <v>30.01</v>
       </c>
       <c r="H17" t="n">
         <v>100</v>
@@ -1092,7 +1098,7 @@
         <v>16</v>
       </c>
       <c r="K17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>